<commit_message>
Only switch left to be placed on schematic
</commit_message>
<xml_diff>
--- a/Mini-ModBot Hardware Integration - Port_Pin Mapping.xlsx
+++ b/Mini-ModBot Hardware Integration - Port_Pin Mapping.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="104">
   <si>
     <t xml:space="preserve">Mini-ModBot Hardware Integration - Port/Pin Mapping </t>
   </si>
@@ -329,9 +329,6 @@
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/c-k-components/1101M2S4AQE2/CKN5050-ND/483720</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/schurter-inc/T9-818C-6/486-3051-ND/4895729</t>
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/PPTC051LFBN-RC/S6103-ND/807239</t>
@@ -2205,8 +2202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -3148,25 +3145,25 @@
         <v>93</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A55" t="s">
+    <row r="55" spans="1:3" s="61" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A55" s="61" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A56" t="s">
+    <row r="56" spans="1:3" s="61" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A56" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="C56" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A57" t="s">
+      <c r="C56" s="61" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" s="61" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A57" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="C57" t="s">
-        <v>104</v>
+      <c r="C57" s="61" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" customHeight="1">
@@ -3174,12 +3171,12 @@
         <v>97</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A59" t="s">
+    <row r="59" spans="1:3" s="61" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A59" s="61" t="s">
         <v>98</v>
       </c>
-      <c r="C59" t="s">
-        <v>103</v>
+      <c r="C59" s="61" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" customHeight="1">
@@ -3190,12 +3187,9 @@
         <v>101</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A61" t="s">
+    <row r="61" spans="1:3" s="61" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A61" s="61" t="s">
         <v>100</v>
-      </c>
-      <c r="C61" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Switch still left. Couple points of feedback from Aparna incorporated.
</commit_message>
<xml_diff>
--- a/Mini-ModBot Hardware Integration - Port_Pin Mapping.xlsx
+++ b/Mini-ModBot Hardware Integration - Port_Pin Mapping.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="110">
   <si>
     <t xml:space="preserve">Mini-ModBot Hardware Integration - Port/Pin Mapping </t>
   </si>
@@ -335,6 +335,24 @@
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/PPPC031LFBN-RC/S7036-ND/810175</t>
+  </si>
+  <si>
+    <t>Removed decoupling cap on IMU - C1</t>
+  </si>
+  <si>
+    <t>Lidar switch for switching between 3.3V/5V</t>
+  </si>
+  <si>
+    <t>PIC inductor on AVDD/Vss</t>
+  </si>
+  <si>
+    <t>Unused IO pull-down?</t>
+  </si>
+  <si>
+    <t>MCLR connection cap?</t>
+  </si>
+  <si>
+    <t>AREF/IOREF on Edison</t>
   </si>
 </sst>
 </file>
@@ -2200,10 +2218,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB61"/>
+  <dimension ref="A1:AB68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -3192,6 +3210,36 @@
         <v>100</v>
       </c>
     </row>
+    <row r="63" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A63" s="57" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A64" s="57" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A65" s="57" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A66" s="57" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A67" s="57" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A68" s="57" t="s">
+        <v>109</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>

</xml_diff>